<commit_message>
Se añaden capacitores de desacople al SIWA y se actualiza el excel con el archivo BoM
</commit_message>
<xml_diff>
--- a/Sprint 1/BoM.xlsx
+++ b/Sprint 1/BoM.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1282a9ba0c2fde91/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{53D2BFA7-277C-469D-81A8-ADFD2C0339EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{025C863E-69CD-48C6-B144-82ACBC2ED437}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE824E82-930D-4CB3-8115-C04483D5CF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{31353D7F-BC04-4EE5-A824-A956B74CBEF0}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{FB2D4811-2369-4154-8C1D-A2A529354672}"/>
   </bookViews>
   <sheets>
-    <sheet name="partes_proyecto" sheetId="1" r:id="rId1"/>
+    <sheet name="Componentes" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">partes_proyecto!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Componentes!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="130">
   <si>
     <t>Line #</t>
   </si>
@@ -119,6 +119,30 @@
     <t>80-C0805F103K5R</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>CC0805KKX7R7BB105</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 16V X7R 0805</t>
+  </si>
+  <si>
+    <t>C_des_1, C_des_2, C_des_3, C_des_4, C_des_5, C_des_6, C_des_7, C_des_8, C_des_9, C_des_10, C_IN, C_IN3, C_IN4, C_IN_, C_OUT, C_OUT_</t>
+  </si>
+  <si>
+    <t>CMP-03422-000001-1</t>
+  </si>
+  <si>
+    <t>New From Design</t>
+  </si>
+  <si>
+    <t>Yageo Group</t>
+  </si>
+  <si>
+    <t>603-CC805KKX7R7BB105</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
@@ -134,9 +158,6 @@
     <t>CMP-2000-05002-2</t>
   </si>
   <si>
-    <t>New From Design</t>
-  </si>
-  <si>
     <t>Vishay</t>
   </si>
   <si>
@@ -149,27 +170,6 @@
     <t>62AC8337</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>CC0805KKX7R7BB105</t>
-  </si>
-  <si>
-    <t>CAP CER 1UF 16V X7R 0805</t>
-  </si>
-  <si>
-    <t>C_IN, C_IN3, C_IN4, C_IN_, C_OUT, C_OUT_</t>
-  </si>
-  <si>
-    <t>CMP-03422-000001-1</t>
-  </si>
-  <si>
-    <t>Yageo Group</t>
-  </si>
-  <si>
-    <t>603-CC805KKX7R7BB105</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -407,13 +407,7 @@
     <t>Arrow Electronics</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
     <t>74LVC2G17GW,125</t>
-  </si>
-  <si>
-    <t>Buffer, Non-Inverting 2 Element 1 Bit per Element Push-Pull Output 6-TSSOP</t>
   </si>
   <si>
     <t>U4, U5, U7, U8, U9</t>
@@ -830,19 +824,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C82403-D0C1-4DCC-991D-DDB952D07505}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AA7025-8A4A-4151-9A0E-A2D9F4ED2125}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="2" max="4" width="16.33203125" customWidth="1"/>
     <col min="5" max="5" width="12.88671875" customWidth="1"/>
     <col min="6" max="6" width="16.77734375" customWidth="1"/>
     <col min="7" max="7" width="15.88671875" customWidth="1"/>
@@ -973,45 +965,45 @@
         <v>21</v>
       </c>
       <c r="H3" s="1">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>32</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N3" s="1">
-        <v>3.5999999999999997E-2</v>
+        <v>0.05</v>
       </c>
       <c r="O3" s="1">
-        <v>0.18</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>31</v>
@@ -1020,28 +1012,28 @@
         <v>21</v>
       </c>
       <c r="H4" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>42</v>
       </c>
       <c r="N4" s="1">
-        <v>0.05</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="O4" s="1">
-        <v>0.5</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1124,10 +1116,10 @@
         <v>57</v>
       </c>
       <c r="N6" s="1">
-        <v>0.17885999999999999</v>
+        <v>0.17827999999999999</v>
       </c>
       <c r="O6" s="1">
-        <v>1.79</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -1295,7 +1287,7 @@
         <v>8</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>78</v>
@@ -1476,7 +1468,7 @@
         <v>23</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>109</v>
@@ -1566,16 +1558,16 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="2" t="s">
@@ -1595,19 +1587,19 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>20</v>
@@ -1619,10 +1611,10 @@
         <v>1</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>23</v>
@@ -1631,13 +1623,13 @@
         <v>121</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="N18" s="1">
-        <v>9.8699999999999996E-2</v>
+        <v>8.9700000000000002E-2</v>
       </c>
       <c r="O18" s="1">
-        <v>9.8699999999999996E-2</v>
+        <v>8.9700000000000002E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nueva iteración del arreglo del PCB
</commit_message>
<xml_diff>
--- a/Sprint 1/BoM.xlsx
+++ b/Sprint 1/BoM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1282a9ba0c2fde91/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://estudianteccr-my.sharepoint.com/personal/gabo20021228_estudiantec_cr/Documents/Taller_Integrador-Proyecto/Sprint 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE824E82-930D-4CB3-8115-C04483D5CF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{CE824E82-930D-4CB3-8115-C04483D5CF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31B35BEF-780D-4247-A94D-C5729B499DDB}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{FB2D4811-2369-4154-8C1D-A2A529354672}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FB2D4811-2369-4154-8C1D-A2A529354672}"/>
   </bookViews>
   <sheets>
     <sheet name="Componentes" sheetId="1" r:id="rId1"/>
@@ -828,13 +828,15 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="4" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
     <col min="5" max="5" width="12.88671875" customWidth="1"/>
     <col min="6" max="6" width="16.77734375" customWidth="1"/>
     <col min="7" max="7" width="15.88671875" customWidth="1"/>

</xml_diff>